<commit_message>
Add starting address to main function in AddressFinder.py
</commit_message>
<xml_diff>
--- a/addresses_found.xlsx
+++ b/addresses_found.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,631 +450,442 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hangar 107,  107</t>
+          <t>1 Rue du Clos Tellier</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>49.44105625</v>
+        <v>49.377805</v>
       </c>
       <c r="D2" t="n">
-        <v>1.072836054933497</v>
+        <v>1.115311</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.44105625,1.0728360549334974</t>
+          <t>https://www.google.com/maps/place/1+Rue+du+Clos+Tellier</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rue Ambroise Fleury,  Quartier Saint-Marc / Croix de Pierre / Saint-Nicaise</t>
+          <t>Rue Alfred Duthil,  La Girafe</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>49.4379835</v>
+        <v>49.44899691233225</v>
       </c>
       <c r="D3" t="n">
-        <v>1.1026282</v>
+        <v>1.152946525663122</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4379835,1.1026282</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.44899691233225,1.1529465256631215</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Rue Antoine de Saint-Exupéry,  Parc de la Bresle</t>
+          <t>Rue du Four Banal,  Déville-lès-Rouen</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>49.46269885</v>
+        <v>49.46194366399145</v>
       </c>
       <c r="D4" t="n">
-        <v>1.073441601313796</v>
+        <v>1.051755879188496</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.462698849999995,1.0734416013137955</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.46194366399145,1.0517558791884958</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Rue de la Vatine,  La Vatine</t>
+          <t>Centre hospitalier du Rouvray,  4</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>49.47003005995345</v>
+        <v>49.39848725</v>
       </c>
       <c r="D5" t="n">
-        <v>1.097510903008701</v>
+        <v>1.09497675154378</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.47003005995345,1.0975109030087011</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.39848725,1.09497675154378</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Rue Verte,  Quartier Gare / Jouvenet</t>
+          <t>Avenue du Grand Cours,  La Sablière</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>49.4498461</v>
+        <v>49.4260239</v>
       </c>
       <c r="D6" t="n">
-        <v>1.093304711245519</v>
+        <v>1.102107434450814</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4498461,1.0933047112455192</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.426023900000004,1.1021074344508142</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Rue Carnot,  Bihorel</t>
+          <t>Boulevard Maurice de Broglie,  Parc de la Bresle</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>49.45555784972355</v>
+        <v>49.46046790356267</v>
       </c>
       <c r="D7" t="n">
-        <v>1.115504930758006</v>
+        <v>1.073605849279293</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.455557849723554,1.1155049307580065</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.46046790356267,1.073605849279293</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Rue Coquerel,  Mont-Saint-Aignan</t>
+          <t>Foire Saint-Romain,  Presqu'Île Rollet</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>49.4543744251689</v>
+        <v>49.44684465</v>
       </c>
       <c r="D8" t="n">
-        <v>1.085397179695553</v>
+        <v>1.054295428337912</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4543744251689,1.0853971796955535</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.44684465,1.0542954283379116</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Rue Delarue Leroy,  Le Mont Fortin</t>
+          <t>Quai Richard Waddington,  Presqu'Île Rollet</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>49.46246069883718</v>
+        <v>49.4407633</v>
       </c>
       <c r="D9" t="n">
-        <v>1.104309739277101</v>
+        <v>1.0466735</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.462460698837184,1.1043097392771009</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4407633,1.0466735</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Rue François Mitterrand,  Flaubert</t>
+          <t>Rue Michel,  Les Coquets</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>49.4265371</v>
+        <v>49.45709401172554</v>
       </c>
       <c r="D10" t="n">
-        <v>1.0633673</v>
+        <v>1.091581960520784</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4265371,1.0633673</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.457094011725545,1.0915819605207844</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Rue Le Verrier,  Parc de l'Epte</t>
+          <t>Quai de Rouen-Quevilly,  Presqu'Île Rollet</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>49.47007525</v>
+        <v>49.43784023857489</v>
       </c>
       <c r="D11" t="n">
-        <v>1.073631797350675</v>
+        <v>1.052916873215403</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.47007525,1.0736317973506746</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.437840238574886,1.052916873215403</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Pont Flaubert,  Presqu'Île Rollet</t>
+          <t>Rue Ernest Lesueur,  Les Coquets</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>49.44133069999999</v>
+        <v>49.45884816717249</v>
       </c>
       <c r="D12" t="n">
-        <v>1.065146643849046</v>
+        <v>1.085739919873663</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.441330699999995,1.0651466438490456</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.45884816717249,1.0857399198736635</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Rue du Docteur Caron,  Bihorel</t>
+          <t>Chemin de Rouen,  Le Mesnil-Esnard</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>49.46006277822872</v>
+        <v>49.41840144619702</v>
       </c>
       <c r="D13" t="n">
-        <v>1.11188552354585</v>
+        <v>1.144385058694083</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.460062778228725,1.11188552354585</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.418401446197024,1.1443850586940834</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Rue Robert Lehmann,  Parc de Cerisy</t>
+          <t>Rue François Lamy,  Mont-Riboudet</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>49.46942484177057</v>
+        <v>49.4484727</v>
       </c>
       <c r="D14" t="n">
-        <v>1.078109619670695</v>
+        <v>1.0746356</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.46942484177057,1.0781096196706945</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4484727,1.0746356</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Rampe du Brillant Point de Vue,  Le Mont Fortin</t>
+          <t>Hippodrome des Trois Pipes,  Rue de Diane</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>49.45264078329139</v>
+        <v>49.45964395</v>
       </c>
       <c r="D15" t="n">
-        <v>1.100410981769812</v>
+        <v>1.118264972943661</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.45264078329139,1.1004109817698116</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.45964395,1.1182649729436607</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Flaubert,  Le Petit-Quevilly</t>
+          <t>Rue de Verdun,  Les Vikings</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>49.43701457127947</v>
+        <v>49.47553723731352</v>
       </c>
       <c r="D16" t="n">
-        <v>1.068236032743768</v>
+        <v>1.123740339433279</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.43701457127947,1.0682360327437683</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.475537237313524,1.123740339433279</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Allée du Coteau,  Déville-lès-Rouen</t>
+          <t>Chemin de la Bretèque,  La Bretèque</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>49.46249961696202</v>
+        <v>49.4895594</v>
       </c>
       <c r="D17" t="n">
-        <v>1.059169152649343</v>
+        <v>1.1035399</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.46249961696202,1.0591691526493432</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4895594,1.1035399</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Intermarché Super,  64</t>
+          <t>6,  Rue des Canadiens</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>49.44022715</v>
+        <v>49.420784</v>
       </c>
       <c r="D18" t="n">
-        <v>1.148263230757958</v>
+        <v>1.128584978738117</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.44022715,1.1482632307579579</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.420784,1.1285849787381173</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Rue de l'Avenir,  Mont-Saint-Aignan</t>
+          <t>2,  Rue Legouy</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>49.4583074</v>
+        <v>49.4425295</v>
       </c>
       <c r="D19" t="n">
-        <v>1.0936924</v>
+        <v>1.108076</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4583074,1.0936924</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4425295,1.108076</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Rue du Commandant Dubois,  L'Église</t>
+          <t>Avenue Bernard Bicheray,  Rouen</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>49.47006606073975</v>
+        <v>49.44945537954387</v>
       </c>
       <c r="D20" t="n">
-        <v>1.110514608485934</v>
+        <v>1.049347084850659</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.470066060739754,1.1105146084859339</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.44945537954387,1.0493470848506585</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Rue des Canadiens,  Château de Waddington</t>
+          <t>Rue Gessard,  Saint-Clément</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>49.43246902549397</v>
+        <v>49.42722088104083</v>
       </c>
       <c r="D21" t="n">
-        <v>1.14724128255841</v>
+        <v>1.071434974292933</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.432469025493965,1.14724128255841</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.42722088104083,1.0714349742929332</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Rue Louis Antier,  Sotteville-lès-Rouen</t>
+          <t>Rampe Beauvoisine,  Jouvenet</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>49.41396867468393</v>
+        <v>49.44801269803951</v>
       </c>
       <c r="D22" t="n">
-        <v>1.077376030792611</v>
+        <v>1.102314470687749</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.41396867468393,1.077376030792611</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>22</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Square de Mortemer,  La Prévotière</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>49.46188525919403</v>
-      </c>
-      <c r="D23" t="n">
-        <v>1.12112692682898</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.46188525919403,1.1211269268289803</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>23</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Avenue du Grand Cours,  La Sablière</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>49.4260239</v>
-      </c>
-      <c r="D24" t="n">
-        <v>1.102107434450814</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.426023900000004,1.1021074344508142</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Skatepark of Rouen,  1</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>49.4385077</v>
-      </c>
-      <c r="D25" t="n">
-        <v>1.072168991886268</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4385077,1.0721689918862676</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>École élémentaire Louis-Ezechiel Pouchet,  Rue Général Giraud</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>49.440661</v>
-      </c>
-      <c r="D26" t="n">
-        <v>1.0876505</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.440661,1.0876505</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>26</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Ambulances Auvray,  3</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>49.4288915</v>
-      </c>
-      <c r="D27" t="n">
-        <v>1.0693691</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4288915,1.0693691</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>1,  Rue du Renard</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>49.4461271</v>
-      </c>
-      <c r="D28" t="n">
-        <v>1.0858071</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4461271,1.0858071</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Quai Bas Jacques Anquetil,  La Sablière</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>49.43233756771774</v>
-      </c>
-      <c r="D29" t="n">
-        <v>1.097535168718729</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.43233756771774,1.0975351687187287</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Rue Louis Malliot,  Jouvenet</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>49.45037807607455</v>
-      </c>
-      <c r="D30" t="n">
-        <v>1.097291600559886</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.45037807607455,1.0972916005598858</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Quai Lescure,  Amfreville-la-Mi-Voie</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>49.4141241512298</v>
-      </c>
-      <c r="D31" t="n">
-        <v>1.118656421283006</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4141241512298,1.1186564212830057</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.44801269803951,1.102314470687749</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor main function in AddressFinder.py to remove hardcoded starting address
</commit_message>
<xml_diff>
--- a/addresses_found.xlsx
+++ b/addresses_found.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,442 +450,421 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1 Rue du Clos Tellier</t>
+          <t>Route de Darnétal,  Bonsecours</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>49.377805</v>
+        <v>49.4285697</v>
       </c>
       <c r="D2" t="n">
-        <v>1.115311</v>
+        <v>1.1453215</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/1+Rue+du+Clos+Tellier</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4285697,1.1453215</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rue Alfred Duthil,  La Girafe</t>
+          <t>Quartier du Mont Gargan,  Bonsecours</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>49.44899691233225</v>
+        <v>49.42307500911448</v>
       </c>
       <c r="D3" t="n">
-        <v>1.152946525663122</v>
+        <v>1.113333097556789</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.44899691233225,1.1529465256631215</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.423075009114484,1.1133330975567892</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Rue du Four Banal,  Déville-lès-Rouen</t>
+          <t>Rue Madame de Staël,  Le Châtelet</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>49.46194366399145</v>
+        <v>49.4594655</v>
       </c>
       <c r="D4" t="n">
-        <v>1.051755879188496</v>
+        <v>1.1360113</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.46194366399145,1.0517558791884958</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4594655,1.1360113</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Centre hospitalier du Rouvray,  4</t>
+          <t>Rue Bellevue,  Le Mont Fortin</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>49.39848725</v>
+        <v>49.45743925693177</v>
       </c>
       <c r="D5" t="n">
-        <v>1.09497675154378</v>
+        <v>1.09952913611965</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.39848725,1.09497675154378</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.45743925693177,1.0995291361196504</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Avenue du Grand Cours,  La Sablière</t>
+          <t>Quai Richard Waddington,  Presqu'Île Rollet</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>49.4260239</v>
+        <v>49.44372233586422</v>
       </c>
       <c r="D6" t="n">
-        <v>1.102107434450814</v>
+        <v>1.05654883905663</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.426023900000004,1.1021074344508142</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.44372233586422,1.0565488390566298</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Boulevard Maurice de Broglie,  Parc de la Bresle</t>
+          <t>Mosquée El-Fath,  Rue Le Verrier</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>49.46046790356267</v>
+        <v>49.45449635</v>
       </c>
       <c r="D7" t="n">
-        <v>1.073605849279293</v>
+        <v>1.141399220863771</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.46046790356267,1.073605849279293</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.45449635,1.1413992208637707</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Foire Saint-Romain,  Presqu'Île Rollet</t>
+          <t>Stade Irène Hermel,  Allée Jacques Willig</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>49.44684465</v>
+        <v>49.42395645</v>
       </c>
       <c r="D8" t="n">
-        <v>1.054295428337912</v>
+        <v>1.0987216635178</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.44684465,1.0542954283379116</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.42395645,1.0987216635177997</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Quai Richard Waddington,  Presqu'Île Rollet</t>
+          <t>Rue Léonard Bordes,  Quartier du Mont Gargan</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>49.4407633</v>
+        <v>49.4343074</v>
       </c>
       <c r="D9" t="n">
-        <v>1.0466735</v>
+        <v>1.1157783</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4407633,1.0466735</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4343074,1.1157783</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Rue Michel,  Les Coquets</t>
+          <t>Rue de Fontenelle,  Déville-lès-Rouen</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>49.45709401172554</v>
+        <v>49.47296713563828</v>
       </c>
       <c r="D10" t="n">
-        <v>1.091581960520784</v>
+        <v>1.060327903948913</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.457094011725545,1.0915819605207844</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.47296713563828,1.0603279039489126</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Quai de Rouen-Quevilly,  Presqu'Île Rollet</t>
+          <t>La table du Boucher,  3980</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>49.43784023857489</v>
+        <v>49.4747228</v>
       </c>
       <c r="D11" t="n">
-        <v>1.052916873215403</v>
+        <v>1.1256959</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.437840238574886,1.052916873215403</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4747228,1.1256959</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Rue Ernest Lesueur,  Les Coquets</t>
+          <t>Rue Abbé de l'Épée,  Croix de Pierre</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>49.45884816717249</v>
+        <v>49.4428704</v>
       </c>
       <c r="D12" t="n">
-        <v>1.085739919873663</v>
+        <v>1.101857240774189</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.45884816717249,1.0857399198736635</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.442870400000004,1.1018572407741893</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Chemin de Rouen,  Le Mesnil-Esnard</t>
+          <t>Route de Mesnil-Esnard,  Côteaux du Trianon</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>49.41840144619702</v>
+        <v>49.42926201468572</v>
       </c>
       <c r="D13" t="n">
-        <v>1.144385058694083</v>
+        <v>1.152774326633283</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.418401446197024,1.1443850586940834</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.42926201468572,1.1527743266332833</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Rue François Lamy,  Mont-Riboudet</t>
+          <t>Rue Alfred Kastler,  Parc d'activités technologiques La Vatine</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>49.4484727</v>
+        <v>49.47288926551011</v>
       </c>
       <c r="D14" t="n">
-        <v>1.0746356</v>
+        <v>1.096211263258272</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4484727,1.0746356</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.47288926551011,1.0962112632582721</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Hippodrome des Trois Pipes,  Rue de Diane</t>
+          <t>Résidence Muchedent,  Darnétal</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>49.45964395</v>
+        <v>49.4501356</v>
       </c>
       <c r="D15" t="n">
-        <v>1.118264972943661</v>
+        <v>1.1564396</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.45964395,1.1182649729436607</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4501356,1.1564396</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Rue de Verdun,  Les Vikings</t>
+          <t>Rue Henri Frère,  Parc de la Varenne</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>49.47553723731352</v>
+        <v>49.46044837309679</v>
       </c>
       <c r="D16" t="n">
-        <v>1.123740339433279</v>
+        <v>1.066894627953609</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.475537237313524,1.123740339433279</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.46044837309679,1.0668946279536091</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Chemin de la Bretèque,  La Bretèque</t>
+          <t>Rue du Cantony,  Centre Commercial de l'Aubette</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>49.4895594</v>
+        <v>49.43451528263126</v>
       </c>
       <c r="D17" t="n">
-        <v>1.1035399</v>
+        <v>1.155047846947832</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4895594,1.1035399</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.43451528263126,1.1550478469478322</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>6,  Rue des Canadiens</t>
+          <t>Pont Flaubert,  Quai de France</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>49.420784</v>
+        <v>49.44133069999999</v>
       </c>
       <c r="D18" t="n">
-        <v>1.128584978738117</v>
+        <v>1.065146643849046</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.420784,1.1285849787381173</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.441330699999995,1.0651466438490456</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2,  Rue Legouy</t>
+          <t>Chemin de la Grand'Mare,  Vallon Suisse</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>49.4425295</v>
+        <v>49.45606676013594</v>
       </c>
       <c r="D19" t="n">
-        <v>1.108076</v>
+        <v>1.134587443855071</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.4425295,1.108076</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.45606676013594,1.134587443855071</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Avenue Bernard Bicheray,  Rouen</t>
+          <t>Boulevard Industriel,  Sotteville-lès-Rouen</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>49.44945537954387</v>
+        <v>49.40399859811959</v>
       </c>
       <c r="D20" t="n">
-        <v>1.049347084850659</v>
+        <v>1.110365343518302</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.44945537954387,1.0493470848506585</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.40399859811959,1.110365343518302</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Rue Gessard,  Saint-Clément</t>
+          <t>Rue de l'Appel du 18 Juin 1940,  La Prévotière</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>49.42722088104083</v>
+        <v>49.46639417381033</v>
       </c>
       <c r="D21" t="n">
-        <v>1.071434974292933</v>
+        <v>1.12582431140331</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.42722088104083,1.0714349742929332</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Rampe Beauvoisine,  Jouvenet</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>49.44801269803951</v>
-      </c>
-      <c r="D22" t="n">
-        <v>1.102314470687749</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/search/?api=1&amp;query=49.44801269803951,1.102314470687749</t>
+          <t>https://www.google.com/maps/search/?api=1&amp;query=49.46639417381033,1.1258243114033095</t>
         </is>
       </c>
     </row>

</xml_diff>